<commit_message>
Ajout des nouveaux profils au flux 1 26a60a771d9326b9757545557df9a6e89fe243f4
</commit_message>
<xml_diff>
--- a/361-Flux-Mise-à-jour-du-flux-1/ig/CodeSystem-input-tddui-task-transport-codesystem.xlsx
+++ b/361-Flux-Mise-à-jour-du-flux-1/ig/CodeSystem-input-tddui-task-transport-codesystem.xlsx
@@ -30,7 +30,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>2.0.0-ballot</t>
+    <t>2.0.0</t>
   </si>
   <si>
     <t>Name</t>
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-10-01T08:29:05+00:00</t>
+    <t>2025-10-20T13:10:23+00:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>